<commit_message>
atualizacao do backlog da sprint 2
</commit_message>
<xml_diff>
--- a/docs/Arquivos_técnicos/Product Backlog + sprint backlog.xlsx
+++ b/docs/Arquivos_técnicos/Product Backlog + sprint backlog.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caio\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Desktop\a\API-2023.1\docs\Arquivos_técnicos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F055DEBD-106D-430E-825E-27BC1EB8FCC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1D65B229-CEEC-4294-8C83-681DF19FC769}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Backlog geral" sheetId="1" r:id="rId1"/>
+    <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Backlog sprint 2" sheetId="3" r:id="rId2"/>
     <sheet name="Backlog sprint 3" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="102">
   <si>
     <t>ID</t>
   </si>
@@ -223,27 +222,15 @@
     <t>Tempo para conclusão</t>
   </si>
   <si>
-    <t>Pegar os dados arrecadados e comparar a taxa de aumento e diminuição em relação ao anos</t>
-  </si>
-  <si>
     <t>Desenvolver a logo</t>
   </si>
   <si>
-    <t>Desenvolver  navbar e rodapé</t>
-  </si>
-  <si>
     <t>Apresentação e roteiro</t>
   </si>
   <si>
     <t>Criar a página Home, de acordo com o wireframe</t>
   </si>
   <si>
-    <t>Criar a página Pesquisa, de acordo com o wireframe</t>
-  </si>
-  <si>
-    <t>Criar a página Sobre o projeto, de acordo com o wireframe</t>
-  </si>
-  <si>
     <t>Prioridade</t>
   </si>
   <si>
@@ -301,46 +288,67 @@
     <t>Desenvolvimento do BD</t>
   </si>
   <si>
-    <t>Informações no site</t>
-  </si>
-  <si>
-    <t>Adicionar as informações(textos, mapas, dados, etc) às páginas</t>
-  </si>
-  <si>
-    <t>Eu, como usuário, quero poder ver a porcetagem de aumento ou diminuição sobre um certos dados de acordo com os anos</t>
-  </si>
-  <si>
-    <t>2 dias</t>
-  </si>
-  <si>
     <t>1 dia</t>
   </si>
   <si>
     <t>1 hora</t>
   </si>
   <si>
-    <t>3 dias</t>
-  </si>
-  <si>
     <t>2~3 dias</t>
   </si>
   <si>
     <t>1 Hora</t>
   </si>
   <si>
-    <t>Estruturar e estilizar pág. Home</t>
-  </si>
-  <si>
-    <t>Estruturar e estilizar pag. Pesquisa</t>
-  </si>
-  <si>
-    <t>Estruturar e estilizar pág. Sobre o projeto</t>
+    <t>Desenvolver uma base do protótipo para ser usada em outras páginas</t>
+  </si>
+  <si>
+    <t>Organização e criação do necessário para desenvolver as páginas no FLASK</t>
+  </si>
+  <si>
+    <t>Informações no protótipo</t>
+  </si>
+  <si>
+    <t>Adicionar ao FIGMA, os textos, gráfico e informações que estarão no site</t>
+  </si>
+  <si>
+    <t>Desenvolver  barra de navegação e rodapé</t>
+  </si>
+  <si>
+    <t>Protótipo navegável - base (flask)</t>
+  </si>
+  <si>
+    <t>Protótipo navegável - Pesquisa</t>
+  </si>
+  <si>
+    <t>Protótipo navegável - sobre o projeto</t>
+  </si>
+  <si>
+    <t>Utilizar a base do protótipo para desenvolver a página "sobre o projeto"</t>
+  </si>
+  <si>
+    <t>Dev story</t>
+  </si>
+  <si>
+    <t>Utilizar a base  do protótipo para desenvolver a página "pesquisa"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eu, como integrante do projeto, devo desenvolver o conteúdo da página "" com base no Flask (%blocks% do flask) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eu, como integrante do projeto, devo desenvolver a base das páginas, com base no Flask (%blocks% do flask) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eu, como integrante do projeto, devo desenvolver o conteúdo da página "pesquisa" com base no Flask (%blocks% do flask) </t>
+  </si>
+  <si>
+    <t>Eu, como dev, devo criar um arquivo CSS, que será referenciado em todas as páginas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -599,71 +607,99 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="60% - Ênfase3" xfId="4" builtinId="40"/>
     <cellStyle name="Bom" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutro" xfId="3" builtinId="28"/>
+    <cellStyle name="Incorreto" xfId="2" builtinId="27"/>
+    <cellStyle name="Neutra" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Ruim" xfId="2" builtinId="27"/>
     <cellStyle name="Saída" xfId="5" builtinId="21"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -971,11 +1007,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BCDEB3B-803A-4C81-A943-2CA6BDE81633}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -989,10 +1025,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="12"/>
+      <c r="C1" s="28"/>
     </row>
     <row r="2" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -1079,7 +1115,7 @@
       <c r="D13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="27"/>
+      <c r="E13" s="25"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -1094,7 +1130,7 @@
       <c r="D14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="27"/>
+      <c r="E14" s="25"/>
     </row>
     <row r="15" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -1109,7 +1145,7 @@
       <c r="D15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="27"/>
+      <c r="E15" s="25"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -1124,7 +1160,7 @@
       <c r="D16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="27"/>
+      <c r="E16" s="25"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
@@ -1139,7 +1175,7 @@
       <c r="D17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="27"/>
+      <c r="E17" s="25"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
@@ -1154,7 +1190,7 @@
       <c r="D18" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="27"/>
+      <c r="E18" s="25"/>
     </row>
     <row r="19" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
@@ -1169,7 +1205,7 @@
       <c r="D19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="27"/>
+      <c r="E19" s="25"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -1184,7 +1220,7 @@
       <c r="D20" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="28"/>
+      <c r="E20" s="26"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -1199,7 +1235,7 @@
       <c r="D21" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="28"/>
+      <c r="E21" s="26"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -1214,7 +1250,7 @@
       <c r="D22" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="28"/>
+      <c r="E22" s="26"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
@@ -1229,7 +1265,7 @@
       <c r="D23" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="28"/>
+      <c r="E23" s="26"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
@@ -1242,17 +1278,17 @@
       <c r="D24" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="28"/>
+      <c r="E24" s="26"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="28"/>
+      <c r="E25" s="26"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E26" s="28"/>
+      <c r="E26" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1264,11 +1300,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44C9FE3E-92A3-43D8-B81C-6E810D3511B3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1276,175 +1312,173 @@
     <col min="1" max="1" width="20.85546875" style="9" customWidth="1"/>
     <col min="2" max="2" width="45.85546875" style="9" customWidth="1"/>
     <col min="3" max="3" width="54.85546875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="9" customWidth="1"/>
     <col min="6" max="6" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="20" t="s">
+      <c r="C2" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="84" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="21"/>
+      <c r="E6" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="84" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="21"/>
+      <c r="E7" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="21"/>
+      <c r="E8" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="42" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="42" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="42" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="E4" s="25" t="s">
+      <c r="B12" s="20" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="42" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="42" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="42" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="42" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="E12" s="24" t="s">
+      <c r="C12" s="20"/>
+      <c r="D12" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="22" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1455,7 +1489,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCCCAF96-15DC-4BFD-8EEA-872DA90F7D3B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -1464,101 +1498,101 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" style="21" customWidth="1"/>
-    <col min="2" max="2" width="47.42578125" style="21" customWidth="1"/>
-    <col min="3" max="3" width="39" style="21" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" style="21" customWidth="1"/>
-    <col min="5" max="5" width="39" style="21" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" style="19" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="39" style="19" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="19" customWidth="1"/>
+    <col min="5" max="5" width="39" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>68</v>
+      <c r="E2" s="14" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18"/>
+      <c r="A3" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="17"/>
     </row>
     <row r="4" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="16" t="s">
+      <c r="A4" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="18" t="s">
-        <v>69</v>
-      </c>
     </row>
     <row r="5" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="18" t="s">
-        <v>69</v>
+      <c r="A5" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="17" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B8" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="23"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="21"/>
       <c r="E8" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adicao dos backlogs da sprint 1 e 4 + lista com todas as atividades do projeto na documentacao do product backlog
</commit_message>
<xml_diff>
--- a/docs/Arquivos_técnicos/Product Backlog + sprint backlog.xlsx
+++ b/docs/Arquivos_técnicos/Product Backlog + sprint backlog.xlsx
@@ -1,43 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Desktop\a\API-2023.1\docs\Arquivos_técnicos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caio2\OneDrive\Área de Trabalho\API\docs\Arquivos_técnicos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41E4281-394A-49D4-B7D9-038071F5EC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Backlog sprint 2" sheetId="3" r:id="rId2"/>
-    <sheet name="Backlog sprint 3" sheetId="4" r:id="rId3"/>
+    <sheet name="Backlog sprint 1" sheetId="5" r:id="rId2"/>
+    <sheet name="Backlog sprint 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Backlog sprint 3" sheetId="4" r:id="rId4"/>
+    <sheet name="Backlog sprint 4" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="128">
   <si>
     <t>ID</t>
   </si>
@@ -343,12 +335,90 @@
   </si>
   <si>
     <t>Eu, como dev, devo criar um arquivo CSS, que será referenciado em todas as páginas</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Pesquisa consultas</t>
+  </si>
+  <si>
+    <t>Pesquisar sobre consulta realizadas no periodo entre 2019 e 2022</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Pesquisa covid-longa</t>
+  </si>
+  <si>
+    <t>Pesquisar sobre covid-longa e seus sintomas</t>
+  </si>
+  <si>
+    <t>Pesquisa financeira</t>
+  </si>
+  <si>
+    <t>Pesquisar sobre investimentos e gastos com a pandemia nos estados escolhidos, durante o periodo de 2019 até 2022</t>
+  </si>
+  <si>
+    <t>Pesquisa medicamentos</t>
+  </si>
+  <si>
+    <t>Pesquisar sobre medicamentos utilizados contra acovid e covid-longa durante a pandemia</t>
+  </si>
+  <si>
+    <t>Pesquisa procedimentos</t>
+  </si>
+  <si>
+    <t>Pesquisar sobre procedimentos realizados contra a covid e covid longa durante o período de 2019 até 2022</t>
+  </si>
+  <si>
+    <t>Pesquisa saúde-mental</t>
+  </si>
+  <si>
+    <t>Pesquisar sobre a venda de  medicamentos relacionados com depressão durante a pandemia</t>
+  </si>
+  <si>
+    <t>Pesquisa tratamentos</t>
+  </si>
+  <si>
+    <t>Pesquisar sobre hospitalizações e vacinações durante a pandemia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sprint 2</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Criar e adicionar os dados/informações ao BD</t>
+  </si>
+  <si>
+    <t>Refazer a pág. Pesquisa do site</t>
+  </si>
+  <si>
+    <t>Refazer a página para acomodar a integração</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>TESTES</t>
+  </si>
+  <si>
+    <t>Assegurar que o site e BD estão funcionando de acordo</t>
+  </si>
+  <si>
+    <t>Responsividade</t>
+  </si>
+  <si>
+    <t>Atualizar o CSS para garantir que o site fique responsivo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -472,7 +542,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -511,8 +581,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -563,6 +639,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -572,7 +657,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -646,28 +731,31 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="60% - Ênfase3" xfId="4" builtinId="40"/>
     <cellStyle name="Bom" xfId="1" builtinId="26"/>
-    <cellStyle name="Incorreto" xfId="2" builtinId="27"/>
-    <cellStyle name="Neutra" xfId="3" builtinId="28"/>
+    <cellStyle name="Neutro" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Ruim" xfId="2" builtinId="27"/>
     <cellStyle name="Saída" xfId="5" builtinId="21"/>
   </cellStyles>
   <dxfs count="2">
@@ -695,7 +783,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1007,30 +1095,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView zoomScale="42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="139.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="1" customWidth="1"/>
-    <col min="7" max="8" width="29.42578125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="8.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="139.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="29.44140625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="28" t="s">
         <v>53</v>
       </c>
       <c r="C1" s="28"/>
     </row>
-    <row r="2" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>42</v>
       </c>
@@ -1038,7 +1126,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>39</v>
       </c>
@@ -1046,7 +1134,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>44</v>
       </c>
@@ -1054,7 +1142,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>48</v>
       </c>
@@ -1062,7 +1150,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>49</v>
       </c>
@@ -1070,7 +1158,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>50</v>
       </c>
@@ -1078,7 +1166,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>51</v>
       </c>
@@ -1086,8 +1174,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>0</v>
       </c>
@@ -1102,7 +1190,7 @@
       </c>
       <c r="E12"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1117,7 +1205,7 @@
       </c>
       <c r="E13" s="25"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1132,7 +1220,7 @@
       </c>
       <c r="E14" s="25"/>
     </row>
-    <row r="15" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1147,7 +1235,7 @@
       </c>
       <c r="E15" s="25"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1162,7 +1250,7 @@
       </c>
       <c r="E16" s="25"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -1177,7 +1265,7 @@
       </c>
       <c r="E17" s="25"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -1192,7 +1280,7 @@
       </c>
       <c r="E18" s="25"/>
     </row>
-    <row r="19" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
@@ -1207,7 +1295,7 @@
       </c>
       <c r="E19" s="25"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -1220,9 +1308,8 @@
       <c r="D20" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="26"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
@@ -1235,9 +1322,8 @@
       <c r="D21" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="26"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
@@ -1250,9 +1336,8 @@
       <c r="D22" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="26"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>32</v>
       </c>
@@ -1265,9 +1350,8 @@
       <c r="D23" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="26"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>56</v>
       </c>
@@ -1278,21 +1362,350 @@
       <c r="D24" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="26"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="26"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E26" s="26"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+    </row>
+    <row r="29" spans="1:5" ht="84" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="84" x14ac:dyDescent="0.3">
+      <c r="A30" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="126" x14ac:dyDescent="0.3">
+      <c r="A31" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="105" x14ac:dyDescent="0.3">
+      <c r="A32" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="126" x14ac:dyDescent="0.3">
+      <c r="A33" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="126" x14ac:dyDescent="0.3">
+      <c r="A34" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="105" x14ac:dyDescent="0.3">
+      <c r="A35" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+    </row>
+    <row r="37" spans="1:4" ht="84" x14ac:dyDescent="0.3">
+      <c r="A37" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="20"/>
+      <c r="D37" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="210" x14ac:dyDescent="0.3">
+      <c r="A38" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="105" x14ac:dyDescent="0.3">
+      <c r="A39" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" s="20"/>
+      <c r="D39" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="147" x14ac:dyDescent="0.3">
+      <c r="A40" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="D40" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="126" x14ac:dyDescent="0.3">
+      <c r="A41" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="168" x14ac:dyDescent="0.3">
+      <c r="A42" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="84" x14ac:dyDescent="0.3">
+      <c r="A43" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="20"/>
+      <c r="D43" s="26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="105" x14ac:dyDescent="0.3">
+      <c r="A44" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" s="20"/>
+      <c r="D44" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="105" x14ac:dyDescent="0.3">
+      <c r="A45" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" s="20"/>
+      <c r="D45" s="22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="105" x14ac:dyDescent="0.3">
+      <c r="A46" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C46" s="20"/>
+      <c r="D46" s="22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
+    </row>
+    <row r="48" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A48" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C48" s="15"/>
+      <c r="D48" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="54" x14ac:dyDescent="0.3">
+      <c r="A49" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" s="15"/>
+      <c r="D49" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+      <c r="A50" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C50" s="15"/>
+      <c r="D50" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="108" x14ac:dyDescent="0.3">
+      <c r="A51" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C51" s="15"/>
+      <c r="D51" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="B52" s="29"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+    </row>
+    <row r="53" spans="1:4" ht="63" x14ac:dyDescent="0.3">
+      <c r="A53" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B53" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53" s="20"/>
+      <c r="D53" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="63" x14ac:dyDescent="0.3">
+      <c r="A54" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="B54" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C54" s="20"/>
+      <c r="D54" s="23" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A52:D52"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1300,41 +1713,174 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F96868C-B478-4280-A1FA-401ECF2ECB2D}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="39.21875" customWidth="1"/>
+    <col min="2" max="2" width="59.77734375" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="34" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="54.85546875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.88671875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="45.88671875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="54.88671875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="9" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+    <row r="2" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="27" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="63" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>55</v>
       </c>
@@ -1347,7 +1893,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="84" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="84" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>91</v>
       </c>
@@ -1364,7 +1910,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="63" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>89</v>
       </c>
@@ -1377,7 +1923,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>92</v>
       </c>
@@ -1392,7 +1938,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="84" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="84" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>93</v>
       </c>
@@ -1407,7 +1953,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="63" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>94</v>
       </c>
@@ -1422,7 +1968,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="42" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>61</v>
       </c>
@@ -1433,11 +1979,11 @@
       <c r="D9" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="26" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>62</v>
       </c>
@@ -1452,7 +1998,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="63" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>67</v>
       </c>
@@ -1467,7 +2013,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="42" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>68</v>
       </c>
@@ -1488,25 +2034,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" style="19" customWidth="1"/>
-    <col min="2" max="2" width="47.42578125" style="19" customWidth="1"/>
+    <col min="1" max="1" width="31.5546875" style="19" customWidth="1"/>
+    <col min="2" max="2" width="47.44140625" style="19" customWidth="1"/>
     <col min="3" max="3" width="39" style="19" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" style="19" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" style="19" customWidth="1"/>
     <col min="5" max="5" width="39" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
         <v>57</v>
       </c>
@@ -1523,7 +2069,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>82</v>
       </c>
@@ -1532,7 +2078,7 @@
       <c r="D3" s="16"/>
       <c r="E3" s="17"/>
     </row>
-    <row r="4" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>80</v>
       </c>
@@ -1545,7 +2091,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>81</v>
       </c>
@@ -1556,7 +2102,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>73</v>
       </c>
@@ -1569,7 +2115,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>75</v>
       </c>
@@ -1582,7 +2128,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>77</v>
       </c>
@@ -1595,12 +2141,68 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64C2D034-61AD-4D6E-B9B1-E46ABD1C4081}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="4" width="40.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Adicionando novos itens a sprint 3
</commit_message>
<xml_diff>
--- a/docs/Arquivos_técnicos/Product Backlog + sprint backlog.xlsx
+++ b/docs/Arquivos_técnicos/Product Backlog + sprint backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caio2\OneDrive\Área de Trabalho\API\docs\Arquivos_técnicos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caio\Desktop\API\docs\Arquivos_técnicos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41E4281-394A-49D4-B7D9-038071F5EC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D135D813-7DB8-4EBC-BEF1-72594210BFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="133">
   <si>
     <t>ID</t>
   </si>
@@ -208,9 +208,6 @@
     <t>Descrição</t>
   </si>
   <si>
-    <t>User story</t>
-  </si>
-  <si>
     <t>Tempo para conclusão</t>
   </si>
   <si>
@@ -220,9 +217,6 @@
     <t>Apresentação e roteiro</t>
   </si>
   <si>
-    <t>Criar a página Home, de acordo com o wireframe</t>
-  </si>
-  <si>
     <t>Prioridade</t>
   </si>
   <si>
@@ -250,12 +244,6 @@
     <t>Criar uma logo para o site do projeto</t>
   </si>
   <si>
-    <t>Estudo de Flask</t>
-  </si>
-  <si>
-    <t>Estudar a sua funcionalidade e como pode ser aplicado no projeto</t>
-  </si>
-  <si>
     <t>Estudar SQL</t>
   </si>
   <si>
@@ -271,27 +259,9 @@
     <t>Atualizar a documentação e readme de acordo com as mudanças e adições dessa sprint</t>
   </si>
   <si>
-    <t>Integrar com o site</t>
-  </si>
-  <si>
-    <t>Adição dos dados ao site</t>
-  </si>
-  <si>
     <t>Desenvolvimento do BD</t>
   </si>
   <si>
-    <t>1 dia</t>
-  </si>
-  <si>
-    <t>1 hora</t>
-  </si>
-  <si>
-    <t>2~3 dias</t>
-  </si>
-  <si>
-    <t>1 Hora</t>
-  </si>
-  <si>
     <t>Desenvolver uma base do protótipo para ser usada em outras páginas</t>
   </si>
   <si>
@@ -413,13 +383,58 @@
   </si>
   <si>
     <t>Atualizar o CSS para garantir que o site fique responsivo</t>
+  </si>
+  <si>
+    <t>Estudo de Python3</t>
+  </si>
+  <si>
+    <t>Estudo de como será feita a integração/consulta do banco de dados com o site através do Python3</t>
+  </si>
+  <si>
+    <t>Integração com o site</t>
+  </si>
+  <si>
+    <t>Fazer o necessário para integrar/consultar o banco de dados, pelo site, através dos Python3</t>
+  </si>
+  <si>
+    <t>Banco de Dados</t>
+  </si>
+  <si>
+    <t>Desenvolvimento de um BD, para guardar informações das pesquisas e ajudar no filtro de pesquisa</t>
+  </si>
+  <si>
+    <t>Fazer as pesquisas sobre os medicamentos apontados na reunião com jornalista</t>
+  </si>
+  <si>
+    <t>Pesquisa sintomas da covid longa e tratamentos</t>
+  </si>
+  <si>
+    <t>Procurar os sintomas pós-covid e como são tratados(cirurgias, uso de remedios, etc)</t>
+  </si>
+  <si>
+    <t>Pesquisa investimentos</t>
+  </si>
+  <si>
+    <t>Procurar mais fontes sobre e investimentos, na área da saúde, de cada estado escolhido para o projeto(ou a falta deles)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Responsividade </t>
+  </si>
+  <si>
+    <t>Atualizar o CSS para que se adapte para qualquer tamanho de tela sem quebrar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filtros de imagem </t>
+  </si>
+  <si>
+    <t>Atualizar o HTML e CSS, de forma que, as imagens disponibilizadas sejam de diferentes tamanhos e peso para telas diferentes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -479,14 +494,6 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -657,7 +664,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -698,46 +705,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
@@ -747,6 +742,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1102,23 +1100,23 @@
       <selection activeCell="A28" sqref="A28:D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="139.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.44140625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="29.44140625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="139.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="1" customWidth="1"/>
+    <col min="7" max="8" width="29.42578125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="28" t="s">
+    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="28"/>
-    </row>
-    <row r="2" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="24"/>
+    </row>
+    <row r="2" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>42</v>
       </c>
@@ -1126,7 +1124,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>39</v>
       </c>
@@ -1134,7 +1132,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>44</v>
       </c>
@@ -1142,7 +1140,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>48</v>
       </c>
@@ -1150,7 +1148,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>49</v>
       </c>
@@ -1158,7 +1156,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>50</v>
       </c>
@@ -1166,7 +1164,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>51</v>
       </c>
@@ -1174,8 +1172,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>0</v>
       </c>
@@ -1190,7 +1188,7 @@
       </c>
       <c r="E12"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1203,9 +1201,9 @@
       <c r="D13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="25"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E13" s="21"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1218,9 +1216,9 @@
       <c r="D14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="25"/>
-    </row>
-    <row r="15" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="E14" s="21"/>
+    </row>
+    <row r="15" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1233,9 +1231,9 @@
       <c r="D15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="25"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E15" s="21"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1248,9 +1246,9 @@
       <c r="D16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="25"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E16" s="21"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -1263,9 +1261,9 @@
       <c r="D17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="25"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E17" s="21"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -1278,9 +1276,9 @@
       <c r="D18" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="25"/>
-    </row>
-    <row r="19" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="E18" s="21"/>
+    </row>
+    <row r="19" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
@@ -1293,9 +1291,9 @@
       <c r="D19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="25"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E19" s="21"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -1309,7 +1307,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
@@ -1323,7 +1321,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
@@ -1337,7 +1335,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>32</v>
       </c>
@@ -1351,7 +1349,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>56</v>
       </c>
@@ -1363,340 +1361,340 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="29" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+    </row>
+    <row r="29" spans="1:5" ht="84" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="84" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="126" x14ac:dyDescent="0.25">
+      <c r="A31" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="126" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-    </row>
-    <row r="29" spans="1:5" ht="84" x14ac:dyDescent="0.3">
-      <c r="A29" s="20" t="s">
+      <c r="B33" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="C33" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="126" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="B34" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="D29" s="23" t="s">
+      <c r="C34" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+    </row>
+    <row r="37" spans="1:4" ht="84" x14ac:dyDescent="0.25">
+      <c r="A37" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="17"/>
+      <c r="D37" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A39" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="17"/>
+      <c r="D39" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="126" x14ac:dyDescent="0.25">
+      <c r="A40" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="126" x14ac:dyDescent="0.25">
+      <c r="A41" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="168" x14ac:dyDescent="0.25">
+      <c r="A42" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="84" x14ac:dyDescent="0.25">
+      <c r="A43" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" s="17"/>
+      <c r="D43" s="22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A44" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" s="17"/>
+      <c r="D44" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A45" s="17" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="84" x14ac:dyDescent="0.3">
-      <c r="A30" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="B30" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="C30" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D30" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="126" x14ac:dyDescent="0.3">
-      <c r="A31" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="B31" s="20" t="s">
+      <c r="B45" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" s="17"/>
+      <c r="D45" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A46" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C46" s="17"/>
+      <c r="D46" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="C31" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D31" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="105" x14ac:dyDescent="0.3">
-      <c r="A32" s="20" t="s">
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+    </row>
+    <row r="48" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B48" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="C48" s="14"/>
+      <c r="D48" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A49" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C49" s="14"/>
+      <c r="D49" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A50" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" s="14"/>
+      <c r="D50" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="C32" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D32" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="126" x14ac:dyDescent="0.3">
-      <c r="A33" s="20" t="s">
+      <c r="B51" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="B33" s="20" t="s">
+      <c r="C51" s="14"/>
+      <c r="D51" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="C33" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D33" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="126" x14ac:dyDescent="0.3">
-      <c r="A34" s="20" t="s">
+      <c r="B52" s="25"/>
+      <c r="C52" s="25"/>
+      <c r="D52" s="25"/>
+    </row>
+    <row r="53" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A53" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B53" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="C34" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D34" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="105" x14ac:dyDescent="0.3">
-      <c r="A35" s="20" t="s">
+      <c r="C53" s="17"/>
+      <c r="D53" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A54" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B54" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="C35" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D35" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="B36" s="29"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-    </row>
-    <row r="37" spans="1:4" ht="84" x14ac:dyDescent="0.3">
-      <c r="A37" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B37" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="C37" s="20"/>
-      <c r="D37" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="210" x14ac:dyDescent="0.3">
-      <c r="A38" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="B38" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="C38" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="D38" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="105" x14ac:dyDescent="0.3">
-      <c r="A39" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="B39" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="C39" s="20"/>
-      <c r="D39" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="147" x14ac:dyDescent="0.3">
-      <c r="A40" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="B40" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="C40" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="D40" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="126" x14ac:dyDescent="0.3">
-      <c r="A41" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B41" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="C41" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="D41" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="168" x14ac:dyDescent="0.3">
-      <c r="A42" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="B42" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C42" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="D42" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="84" x14ac:dyDescent="0.3">
-      <c r="A43" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B43" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="C43" s="20"/>
-      <c r="D43" s="26" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="105" x14ac:dyDescent="0.3">
-      <c r="A44" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="B44" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="C44" s="20"/>
-      <c r="D44" s="18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="105" x14ac:dyDescent="0.3">
-      <c r="A45" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B45" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="C45" s="20"/>
-      <c r="D45" s="22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="105" x14ac:dyDescent="0.3">
-      <c r="A46" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B46" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="C46" s="20"/>
-      <c r="D46" s="22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="B47" s="30"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-    </row>
-    <row r="48" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A48" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="B48" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="54" x14ac:dyDescent="0.3">
-      <c r="A49" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C49" s="15"/>
-      <c r="D49" s="17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="144" x14ac:dyDescent="0.3">
-      <c r="A50" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="C50" s="15"/>
-      <c r="D50" s="17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="108" x14ac:dyDescent="0.3">
-      <c r="A51" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="C51" s="15"/>
-      <c r="D51" s="18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="B52" s="29"/>
-      <c r="C52" s="29"/>
-      <c r="D52" s="29"/>
-    </row>
-    <row r="53" spans="1:4" ht="63" x14ac:dyDescent="0.3">
-      <c r="A53" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="B53" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="C53" s="20"/>
-      <c r="D53" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="63" x14ac:dyDescent="0.3">
-      <c r="A54" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="B54" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="C54" s="20"/>
-      <c r="D54" s="23" t="s">
-        <v>65</v>
+      <c r="C54" s="17"/>
+      <c r="D54" s="20" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1720,124 +1718,124 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.21875" customWidth="1"/>
-    <col min="2" max="2" width="59.77734375" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26.5546875" customWidth="1"/>
+    <col min="1" max="1" width="39.28515625" customWidth="1"/>
+    <col min="2" max="2" width="59.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:4" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="27" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="B3" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="C6" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="67.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="B7" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+      <c r="C7" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B8" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>65</v>
+      <c r="C8" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1849,182 +1847,192 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:E12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="34" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="45.88671875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="54.88671875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="54.85546875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="9" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+    <row r="2" spans="1:5" ht="46.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="D2" s="27" t="s">
+      <c r="C2" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="84" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="84" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="42" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="B9" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="17"/>
+      <c r="D9" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="22" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="63" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="23" t="s">
+    <row r="10" spans="1:5" ht="42" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="17"/>
+      <c r="D10" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="84" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="63" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="84" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="63" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="42" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="E9" s="26" t="s">
+      <c r="B11" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="42" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="42" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="63" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
+      <c r="B12" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="42" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="20"/>
+      <c r="C12" s="17"/>
       <c r="D12" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="E12" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="19" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2038,115 +2046,176 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.5546875" style="19" customWidth="1"/>
-    <col min="2" max="2" width="47.44140625" style="19" customWidth="1"/>
-    <col min="3" max="3" width="39" style="19" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" style="19" customWidth="1"/>
-    <col min="5" max="5" width="39" style="19" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="54.85546875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" style="9" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+    <row r="1" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="17"/>
-    </row>
-    <row r="4" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2154,53 +2223,41 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64C2D034-61AD-4D6E-B9B1-E46ABD1C4081}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="40.5546875" customWidth="1"/>
+    <col min="1" max="4" width="40.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="42" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="42" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="23" t="s">
-        <v>65</v>
+      <c r="C1" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="42" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="20" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualizacao do backlog da sprint 3
</commit_message>
<xml_diff>
--- a/docs/Arquivos_técnicos/Product Backlog + sprint backlog.xlsx
+++ b/docs/Arquivos_técnicos/Product Backlog + sprint backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caio\Desktop\API\docs\Arquivos_técnicos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D135D813-7DB8-4EBC-BEF1-72594210BFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69273C9-ACDE-4A3D-868D-B942FA20DA8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="139">
   <si>
     <t>ID</t>
   </si>
@@ -397,12 +397,6 @@
     <t>Fazer o necessário para integrar/consultar o banco de dados, pelo site, através dos Python3</t>
   </si>
   <si>
-    <t>Banco de Dados</t>
-  </si>
-  <si>
-    <t>Desenvolvimento de um BD, para guardar informações das pesquisas e ajudar no filtro de pesquisa</t>
-  </si>
-  <si>
     <t>Fazer as pesquisas sobre os medicamentos apontados na reunião com jornalista</t>
   </si>
   <si>
@@ -424,10 +418,34 @@
     <t>Atualizar o CSS para que se adapte para qualquer tamanho de tela sem quebrar</t>
   </si>
   <si>
-    <t xml:space="preserve">Filtros de imagem </t>
-  </si>
-  <si>
-    <t>Atualizar o HTML e CSS, de forma que, as imagens disponibilizadas sejam de diferentes tamanhos e peso para telas diferentes</t>
+    <t>perguntar se vale a pena trabalhar copm BD ou CSV</t>
+  </si>
+  <si>
+    <t>BD ou CVS</t>
+  </si>
+  <si>
+    <t>HTML filtros</t>
+  </si>
+  <si>
+    <t>Implementar a página de filtros no site</t>
+  </si>
+  <si>
+    <t>CSS filtros</t>
+  </si>
+  <si>
+    <t>Desenvolver o CSS para estilizar a pág. Filtros</t>
+  </si>
+  <si>
+    <t>Pesquisa sobre outras cidades</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Nome legal para o site</t>
+  </si>
+  <si>
+    <t>Criar um nome legal pro site e refazer a logo</t>
   </si>
 </sst>
 </file>
@@ -735,6 +753,9 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -742,9 +763,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1111,10 +1129,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="25"/>
     </row>
     <row r="2" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -1368,12 +1386,12 @@
       <c r="D25" s="3"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
     </row>
     <row r="29" spans="1:5" ht="84" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
@@ -1474,12 +1492,12 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
     </row>
     <row r="37" spans="1:4" ht="84" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
@@ -1610,12 +1628,12 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="26" t="s">
+      <c r="A47" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="B47" s="26"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
     </row>
     <row r="48" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
@@ -1666,12 +1684,12 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="25" t="s">
+      <c r="A52" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
     </row>
     <row r="53" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
@@ -2046,7 +2064,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2076,7 +2096,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>118</v>
       </c>
@@ -2093,7 +2113,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>120</v>
       </c>
@@ -2110,12 +2130,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>95</v>
@@ -2123,16 +2143,16 @@
       <c r="D5" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>64</v>
+      <c r="E5" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>100</v>
+        <v>133</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>95</v>
@@ -2140,16 +2160,16 @@
       <c r="D6" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>64</v>
+      <c r="E6" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>95</v>
@@ -2163,57 +2183,89 @@
     </row>
     <row r="8" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B11" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E8" s="27" t="s">
+      <c r="C11" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E9" s="27" t="s">
+    <row r="12" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -2223,10 +2275,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64C2D034-61AD-4D6E-B9B1-E46ABD1C4081}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2234,7 +2286,7 @@
     <col min="1" max="4" width="40.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>57</v>
       </c>
@@ -2245,22 +2297,48 @@
         <v>86</v>
       </c>
       <c r="D1" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="23" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="84" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="20" t="s">
-        <v>63</v>
+        <v>119</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualizacao do backlog da sprint 3, esta de acordo com o burndown e com as atividades realizadas nessa sprint
</commit_message>
<xml_diff>
--- a/docs/Arquivos_técnicos/Product Backlog + sprint backlog.xlsx
+++ b/docs/Arquivos_técnicos/Product Backlog + sprint backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caio\Desktop\API\docs\Arquivos_técnicos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caio2\OneDrive\Área de Trabalho\API\docs\Arquivos_técnicos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69273C9-ACDE-4A3D-868D-B942FA20DA8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04075B2C-C8B2-47D2-8FB7-0CEEADDBFAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="148">
   <si>
     <t>ID</t>
   </si>
@@ -391,51 +391,6 @@
     <t>Estudo de como será feita a integração/consulta do banco de dados com o site através do Python3</t>
   </si>
   <si>
-    <t>Integração com o site</t>
-  </si>
-  <si>
-    <t>Fazer o necessário para integrar/consultar o banco de dados, pelo site, através dos Python3</t>
-  </si>
-  <si>
-    <t>Fazer as pesquisas sobre os medicamentos apontados na reunião com jornalista</t>
-  </si>
-  <si>
-    <t>Pesquisa sintomas da covid longa e tratamentos</t>
-  </si>
-  <si>
-    <t>Procurar os sintomas pós-covid e como são tratados(cirurgias, uso de remedios, etc)</t>
-  </si>
-  <si>
-    <t>Pesquisa investimentos</t>
-  </si>
-  <si>
-    <t>Procurar mais fontes sobre e investimentos, na área da saúde, de cada estado escolhido para o projeto(ou a falta deles)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Responsividade </t>
-  </si>
-  <si>
-    <t>Atualizar o CSS para que se adapte para qualquer tamanho de tela sem quebrar</t>
-  </si>
-  <si>
-    <t>perguntar se vale a pena trabalhar copm BD ou CSV</t>
-  </si>
-  <si>
-    <t>BD ou CVS</t>
-  </si>
-  <si>
-    <t>HTML filtros</t>
-  </si>
-  <si>
-    <t>Implementar a página de filtros no site</t>
-  </si>
-  <si>
-    <t>CSS filtros</t>
-  </si>
-  <si>
-    <t>Desenvolver o CSS para estilizar a pág. Filtros</t>
-  </si>
-  <si>
     <t>Pesquisa sobre outras cidades</t>
   </si>
   <si>
@@ -446,13 +401,85 @@
   </si>
   <si>
     <t>Criar um nome legal pro site e refazer a logo</t>
+  </si>
+  <si>
+    <t>CSV</t>
+  </si>
+  <si>
+    <t>Estilizar filtros</t>
+  </si>
+  <si>
+    <t>Criar o CSS para a página dos filtros</t>
+  </si>
+  <si>
+    <t>Transformar os dados arrecadados no excel para .CSV</t>
+  </si>
+  <si>
+    <t>Página filtros</t>
+  </si>
+  <si>
+    <t>Desenvolver o HTML da página Filtros</t>
+  </si>
+  <si>
+    <t>Raspagem de dados</t>
+  </si>
+  <si>
+    <t>Implementar a raspagem de dados dos arquivos .CSV</t>
+  </si>
+  <si>
+    <t>Complementar a pesquisa sobre medicamentos, de acordo com o que foi falado na reunião com o jornalista</t>
+  </si>
+  <si>
+    <t>Pesquisa tratamentos sintomas covid-longa</t>
+  </si>
+  <si>
+    <t>Pesquisar sobre como são tratados os sintomas da covid-longa</t>
+  </si>
+  <si>
+    <t>Banco de dados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criar no MySQL o banco de dados para feedback </t>
+  </si>
+  <si>
+    <t>Formulário</t>
+  </si>
+  <si>
+    <t>Criar HTML da página para formulário do Feedback</t>
+  </si>
+  <si>
+    <t>Estilizar formulário</t>
+  </si>
+  <si>
+    <t>Criar o CSS para a página feedback/formulário</t>
+  </si>
+  <si>
+    <t>Apresentação</t>
+  </si>
+  <si>
+    <t>Fazer uma apresentação para a sprint atual</t>
+  </si>
+  <si>
+    <t>GitHub</t>
+  </si>
+  <si>
+    <t>Organizar o github</t>
+  </si>
+  <si>
+    <t>Ajustar o CSS do site para se adaptar a diferentes telas de desktop</t>
+  </si>
+  <si>
+    <t>Fazer o formulário funcionar</t>
+  </si>
+  <si>
+    <t>Vincular o Banco de Dados ao formulário</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -562,6 +589,14 @@
     <font>
       <sz val="16"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -682,7 +717,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -765,6 +800,7 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="60% - Ênfase3" xfId="4" builtinId="40"/>
@@ -1118,23 +1154,23 @@
       <selection activeCell="A28" sqref="A28:D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="139.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="1" customWidth="1"/>
-    <col min="7" max="8" width="29.42578125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="8.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="139.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="29.44140625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C1" s="25"/>
     </row>
-    <row r="2" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>42</v>
       </c>
@@ -1142,7 +1178,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>39</v>
       </c>
@@ -1150,7 +1186,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>44</v>
       </c>
@@ -1158,7 +1194,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>48</v>
       </c>
@@ -1166,7 +1202,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>49</v>
       </c>
@@ -1174,7 +1210,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>50</v>
       </c>
@@ -1182,7 +1218,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>51</v>
       </c>
@@ -1190,8 +1226,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>0</v>
       </c>
@@ -1206,7 +1242,7 @@
       </c>
       <c r="E12"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1221,7 +1257,7 @@
       </c>
       <c r="E13" s="21"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1236,7 +1272,7 @@
       </c>
       <c r="E14" s="21"/>
     </row>
-    <row r="15" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1251,7 +1287,7 @@
       </c>
       <c r="E15" s="21"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1266,7 +1302,7 @@
       </c>
       <c r="E16" s="21"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -1281,7 +1317,7 @@
       </c>
       <c r="E17" s="21"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -1296,7 +1332,7 @@
       </c>
       <c r="E18" s="21"/>
     </row>
-    <row r="19" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
@@ -1311,7 +1347,7 @@
       </c>
       <c r="E19" s="21"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -1325,7 +1361,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
@@ -1339,7 +1375,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
@@ -1353,7 +1389,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>32</v>
       </c>
@@ -1367,7 +1403,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>56</v>
       </c>
@@ -1379,13 +1415,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="26" t="s">
         <v>92</v>
       </c>
@@ -1393,7 +1429,7 @@
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
     </row>
-    <row r="29" spans="1:5" ht="84" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="84" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
         <v>93</v>
       </c>
@@ -1407,7 +1443,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="84" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="84" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
         <v>96</v>
       </c>
@@ -1421,7 +1457,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="126" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="126" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
         <v>98</v>
       </c>
@@ -1435,7 +1471,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="105" x14ac:dyDescent="0.3">
       <c r="A32" s="17" t="s">
         <v>100</v>
       </c>
@@ -1449,7 +1485,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="126" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="126" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
         <v>102</v>
       </c>
@@ -1463,7 +1499,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="126" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="126" x14ac:dyDescent="0.3">
       <c r="A34" s="17" t="s">
         <v>104</v>
       </c>
@@ -1477,7 +1513,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="105" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
         <v>106</v>
       </c>
@@ -1491,7 +1527,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="26" t="s">
         <v>108</v>
       </c>
@@ -1499,7 +1535,7 @@
       <c r="C36" s="26"/>
       <c r="D36" s="26"/>
     </row>
-    <row r="37" spans="1:4" ht="84" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="84" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
         <v>55</v>
       </c>
@@ -1511,7 +1547,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="210" x14ac:dyDescent="0.3">
       <c r="A38" s="17" t="s">
         <v>81</v>
       </c>
@@ -1525,7 +1561,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="105" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
         <v>79</v>
       </c>
@@ -1537,7 +1573,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="126" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="126" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
         <v>82</v>
       </c>
@@ -1551,7 +1587,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="126" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="126" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
         <v>83</v>
       </c>
@@ -1565,7 +1601,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="168" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="168" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
         <v>84</v>
       </c>
@@ -1579,7 +1615,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="84" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="84" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
         <v>60</v>
       </c>
@@ -1591,7 +1627,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="105" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
         <v>61</v>
       </c>
@@ -1603,7 +1639,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="105" x14ac:dyDescent="0.3">
       <c r="A45" s="17" t="s">
         <v>65</v>
       </c>
@@ -1615,7 +1651,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="84" x14ac:dyDescent="0.3">
       <c r="A46" s="17" t="s">
         <v>66</v>
       </c>
@@ -1627,7 +1663,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="27" t="s">
         <v>109</v>
       </c>
@@ -1635,7 +1671,7 @@
       <c r="C47" s="27"/>
       <c r="D47" s="27"/>
     </row>
-    <row r="48" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A48" s="14" t="s">
         <v>76</v>
       </c>
@@ -1647,7 +1683,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="54" x14ac:dyDescent="0.3">
       <c r="A49" s="14" t="s">
         <v>71</v>
       </c>
@@ -1659,7 +1695,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="144" x14ac:dyDescent="0.3">
       <c r="A50" s="14" t="s">
         <v>73</v>
       </c>
@@ -1671,7 +1707,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="112.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="108" x14ac:dyDescent="0.3">
       <c r="A51" s="14" t="s">
         <v>111</v>
       </c>
@@ -1683,7 +1719,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="26" t="s">
         <v>113</v>
       </c>
@@ -1691,7 +1727,7 @@
       <c r="C52" s="26"/>
       <c r="D52" s="26"/>
     </row>
-    <row r="53" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="63" x14ac:dyDescent="0.3">
       <c r="A53" s="17" t="s">
         <v>114</v>
       </c>
@@ -1703,7 +1739,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="63" x14ac:dyDescent="0.3">
       <c r="A54" s="17" t="s">
         <v>116</v>
       </c>
@@ -1736,15 +1772,15 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.28515625" customWidth="1"/>
-    <col min="2" max="2" width="59.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="1" max="1" width="39.33203125" customWidth="1"/>
+    <col min="2" max="2" width="59.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>57</v>
       </c>
@@ -1758,7 +1794,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>93</v>
       </c>
@@ -1772,7 +1808,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>96</v>
       </c>
@@ -1786,7 +1822,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>98</v>
       </c>
@@ -1800,7 +1836,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>100</v>
       </c>
@@ -1814,7 +1850,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>102</v>
       </c>
@@ -1828,7 +1864,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="67.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="67.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>104</v>
       </c>
@@ -1842,7 +1878,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>106</v>
       </c>
@@ -1869,17 +1905,17 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="54.85546875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.88671875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="45.88671875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="54.88671875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="9" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="46.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>57</v>
       </c>
@@ -1896,7 +1932,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="63" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>55</v>
       </c>
@@ -1911,7 +1947,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="84" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="84" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>81</v>
       </c>
@@ -1928,7 +1964,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="63" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>79</v>
       </c>
@@ -1943,7 +1979,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>82</v>
       </c>
@@ -1960,7 +1996,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="84" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="84" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>83</v>
       </c>
@@ -1977,7 +2013,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="63" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>84</v>
       </c>
@@ -1994,7 +2030,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="42" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>60</v>
       </c>
@@ -2009,7 +2045,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>61</v>
       </c>
@@ -2024,7 +2060,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="63" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>65</v>
       </c>
@@ -2039,7 +2075,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="42" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>66</v>
       </c>
@@ -2062,24 +2098,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="50" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="54.85546875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.88671875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="45.88671875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="54.88671875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="9" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>57</v>
       </c>
@@ -2096,7 +2132,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>118</v>
       </c>
@@ -2113,12 +2149,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>95</v>
@@ -2130,12 +2166,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>95</v>
@@ -2147,12 +2183,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>95</v>
@@ -2164,12 +2200,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>130</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>95</v>
@@ -2177,16 +2213,16 @@
       <c r="D7" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>100</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>95</v>
@@ -2198,12 +2234,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>95</v>
@@ -2215,12 +2251,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>95</v>
@@ -2228,16 +2264,16 @@
       <c r="D10" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="E10" s="24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>128</v>
+        <v>147</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>95</v>
@@ -2245,11 +2281,12 @@
       <c r="D11" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="E11" s="24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="28"/>
+    </row>
+    <row r="12" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>137</v>
       </c>
@@ -2262,14 +2299,98 @@
       <c r="D12" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2281,12 +2402,12 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="40.5703125" customWidth="1"/>
+    <col min="1" max="4" width="40.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>57</v>
       </c>
@@ -2303,7 +2424,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="84" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="84" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>118</v>
       </c>
@@ -2320,9 +2441,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>95</v>
@@ -2334,7 +2455,7 @@
         <v>95</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualizando o product backlog com as atividades da sprint 3
</commit_message>
<xml_diff>
--- a/docs/Arquivos_técnicos/Product Backlog + sprint backlog.xlsx
+++ b/docs/Arquivos_técnicos/Product Backlog + sprint backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caio2\OneDrive\Área de Trabalho\API\docs\Arquivos_técnicos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04075B2C-C8B2-47D2-8FB7-0CEEADDBFAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32457E92-4E5F-494B-A464-22CE72BFBB1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="136">
   <si>
     <t>ID</t>
   </si>
@@ -244,24 +244,9 @@
     <t>Criar uma logo para o site do projeto</t>
   </si>
   <si>
-    <t>Estudar SQL</t>
-  </si>
-  <si>
-    <t>Estudar a linguagem de BD para aplicação na próxima sprint</t>
-  </si>
-  <si>
-    <t>Estudar integração do BD com python 3</t>
-  </si>
-  <si>
-    <t>Estudar como implementar o BD com o site através de python 3, para a próxima sprint</t>
-  </si>
-  <si>
     <t>Atualizar a documentação e readme de acordo com as mudanças e adições dessa sprint</t>
   </si>
   <si>
-    <t>Desenvolvimento do BD</t>
-  </si>
-  <si>
     <t>Desenvolver uma base do protótipo para ser usada em outras páginas</t>
   </si>
   <si>
@@ -361,28 +346,7 @@
     <t>Sprint 3</t>
   </si>
   <si>
-    <t>Criar e adicionar os dados/informações ao BD</t>
-  </si>
-  <si>
-    <t>Refazer a pág. Pesquisa do site</t>
-  </si>
-  <si>
-    <t>Refazer a página para acomodar a integração</t>
-  </si>
-  <si>
-    <t>Sprint 4</t>
-  </si>
-  <si>
-    <t>TESTES</t>
-  </si>
-  <si>
-    <t>Assegurar que o site e BD estão funcionando de acordo</t>
-  </si>
-  <si>
     <t>Responsividade</t>
-  </si>
-  <si>
-    <t>Atualizar o CSS para garantir que o site fique responsivo</t>
   </si>
   <si>
     <t>Estudo de Python3</t>
@@ -479,7 +443,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -532,20 +496,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -717,7 +667,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -758,39 +708,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -800,7 +742,6 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="60% - Ênfase3" xfId="4" builtinId="40"/>
@@ -1148,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView zoomScale="42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:D54"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1160,17 +1101,16 @@
     <col min="2" max="2" width="30.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="139.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="22.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.44140625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="29.44140625" style="9" customWidth="1"/>
+    <col min="6" max="7" width="29.44140625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="25" t="s">
+    <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="25"/>
-    </row>
-    <row r="2" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="23"/>
+    </row>
+    <row r="2" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>42</v>
       </c>
@@ -1178,7 +1118,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>39</v>
       </c>
@@ -1186,7 +1126,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>44</v>
       </c>
@@ -1194,7 +1134,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>48</v>
       </c>
@@ -1202,7 +1142,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>49</v>
       </c>
@@ -1210,7 +1150,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>50</v>
       </c>
@@ -1218,7 +1158,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>51</v>
       </c>
@@ -1226,8 +1166,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>0</v>
       </c>
@@ -1240,9 +1180,8 @@
       <c r="D12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E12"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1255,9 +1194,8 @@
       <c r="D13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="21"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1270,9 +1208,8 @@
       <c r="D14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="21"/>
-    </row>
-    <row r="15" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1285,9 +1222,8 @@
       <c r="D15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="21"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1300,9 +1236,8 @@
       <c r="D16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="21"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -1315,9 +1250,8 @@
       <c r="D17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="21"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -1330,9 +1264,8 @@
       <c r="D18" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="21"/>
-    </row>
-    <row r="19" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
@@ -1345,9 +1278,8 @@
       <c r="D19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="21"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -1361,7 +1293,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
@@ -1375,7 +1307,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
@@ -1389,7 +1321,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>32</v>
       </c>
@@ -1403,7 +1335,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>56</v>
       </c>
@@ -1415,349 +1347,509 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="26" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+    </row>
+    <row r="29" spans="1:4" ht="84" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="84" x14ac:dyDescent="0.3">
+      <c r="A30" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-    </row>
-    <row r="29" spans="1:5" ht="84" x14ac:dyDescent="0.3">
-      <c r="A29" s="17" t="s">
+      <c r="C30" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="126" x14ac:dyDescent="0.3">
+      <c r="A31" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B31" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C31" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="105" x14ac:dyDescent="0.3">
+      <c r="A32" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="D29" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="84" x14ac:dyDescent="0.3">
-      <c r="A30" s="17" t="s">
+      <c r="B32" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="C32" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="126" x14ac:dyDescent="0.3">
+      <c r="A33" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="B33" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="126" x14ac:dyDescent="0.3">
+      <c r="A34" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="105" x14ac:dyDescent="0.3">
+      <c r="A35" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+    </row>
+    <row r="37" spans="1:7" ht="84" x14ac:dyDescent="0.3">
+      <c r="A37" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="15"/>
+      <c r="D37" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="210" x14ac:dyDescent="0.3">
+      <c r="A38" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="105" x14ac:dyDescent="0.3">
+      <c r="A39" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39" s="15"/>
+      <c r="D39" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="126" x14ac:dyDescent="0.3">
+      <c r="A40" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="126" x14ac:dyDescent="0.3">
+      <c r="A41" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="168" x14ac:dyDescent="0.3">
+      <c r="A42" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="84" x14ac:dyDescent="0.3">
+      <c r="A43" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" s="15"/>
+      <c r="D43" s="19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="105" x14ac:dyDescent="0.3">
+      <c r="A44" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" s="15"/>
+      <c r="D44" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="105" x14ac:dyDescent="0.3">
+      <c r="A45" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C45" s="15"/>
+      <c r="D45" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="84" x14ac:dyDescent="0.3">
+      <c r="A46" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C46" s="15"/>
+      <c r="D46" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B47" s="25"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+    </row>
+    <row r="48" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F48"/>
+      <c r="G48"/>
+    </row>
+    <row r="49" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F49" s="22"/>
+      <c r="G49"/>
+    </row>
+    <row r="50" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F50"/>
+      <c r="G50"/>
+    </row>
+    <row r="51" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F51"/>
+      <c r="G51"/>
+    </row>
+    <row r="52" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F52"/>
+      <c r="G52"/>
+    </row>
+    <row r="53" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="D30" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="126" x14ac:dyDescent="0.3">
-      <c r="A31" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="105" x14ac:dyDescent="0.3">
-      <c r="A32" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="126" x14ac:dyDescent="0.3">
-      <c r="A33" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="126" x14ac:dyDescent="0.3">
-      <c r="A34" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="B34" s="17" t="s">
+      <c r="B53" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F53"/>
+      <c r="G53"/>
+    </row>
+    <row r="54" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B54" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F54"/>
+      <c r="G54"/>
+    </row>
+    <row r="55" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B55" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F55"/>
+      <c r="G55"/>
+    </row>
+    <row r="56" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E56" s="22"/>
+      <c r="F56"/>
+      <c r="G56"/>
+    </row>
+    <row r="57" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F57"/>
+      <c r="G57"/>
+    </row>
+    <row r="58" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B58" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F58"/>
+      <c r="G58"/>
+    </row>
+    <row r="59" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F59"/>
+      <c r="G59"/>
+    </row>
+    <row r="60" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F60"/>
+      <c r="G60"/>
+    </row>
+    <row r="61" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D61" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F61"/>
+      <c r="G61"/>
+    </row>
+    <row r="62" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="C34" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="105" x14ac:dyDescent="0.3">
-      <c r="A35" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-    </row>
-    <row r="37" spans="1:4" ht="84" x14ac:dyDescent="0.3">
-      <c r="A37" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" s="17"/>
-      <c r="D37" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="210" x14ac:dyDescent="0.3">
-      <c r="A38" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="105" x14ac:dyDescent="0.3">
-      <c r="A39" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="C39" s="17"/>
-      <c r="D39" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="126" x14ac:dyDescent="0.3">
-      <c r="A40" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="126" x14ac:dyDescent="0.3">
-      <c r="A41" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="168" x14ac:dyDescent="0.3">
-      <c r="A42" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="B42" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="D42" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="84" x14ac:dyDescent="0.3">
-      <c r="A43" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C43" s="17"/>
-      <c r="D43" s="22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="105" x14ac:dyDescent="0.3">
-      <c r="A44" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="B44" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C44" s="17"/>
-      <c r="D44" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="105" x14ac:dyDescent="0.3">
-      <c r="A45" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="B45" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="C45" s="17"/>
-      <c r="D45" s="19" t="s">
+      <c r="B62" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D62" s="21" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="84" x14ac:dyDescent="0.3">
-      <c r="A46" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="C46" s="17"/>
-      <c r="D46" s="19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-    </row>
-    <row r="48" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A48" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B48" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="C48" s="14"/>
-      <c r="D48" s="15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="54" x14ac:dyDescent="0.3">
-      <c r="A49" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C49" s="14"/>
-      <c r="D49" s="15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="144" x14ac:dyDescent="0.3">
-      <c r="A50" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="B50" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="C50" s="14"/>
-      <c r="D50" s="15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="108" x14ac:dyDescent="0.3">
-      <c r="A51" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="B51" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="C51" s="14"/>
-      <c r="D51" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="B52" s="26"/>
-      <c r="C52" s="26"/>
-      <c r="D52" s="26"/>
-    </row>
-    <row r="53" spans="1:4" ht="63" x14ac:dyDescent="0.3">
-      <c r="A53" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="B53" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="C53" s="17"/>
-      <c r="D53" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="63" x14ac:dyDescent="0.3">
-      <c r="A54" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="B54" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="C54" s="17"/>
-      <c r="D54" s="20" t="s">
-        <v>63</v>
-      </c>
+      <c r="F62"/>
+      <c r="G62"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A36:D36"/>
     <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A52:D52"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1781,114 +1873,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" s="23" t="s">
+      <c r="C1" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B4" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C4" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="B5" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="C5" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="B6" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="C6" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="67.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="B7" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="C7" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+      <c r="B8" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="67.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D8" s="20" t="s">
+      <c r="C8" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="18" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1916,177 +2008,177 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="63" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="84" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="63" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="17" t="s">
+      <c r="D4" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="63" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="84" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="84" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="63" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="B7" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="63" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B8" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="84" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+      <c r="C8" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="63" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E8" s="20" t="s">
+      <c r="D8" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="18" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="42" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E9" s="22" t="s">
+      <c r="C9" s="15"/>
+      <c r="D9" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="19" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="42" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E10" s="16" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="63" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E11" s="19" t="s">
+      <c r="B11" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="17" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="42" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="17"/>
+      <c r="C12" s="15"/>
       <c r="D12" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="E12" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" s="17" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2100,8 +2192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="50" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="A6" zoomScale="50" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2116,275 +2208,275 @@
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="23" t="s">
+      <c r="C2" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="20" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B7" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C7" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>95</v>
+      <c r="B8" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>95</v>
+      <c r="A9" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>95</v>
+      <c r="A10" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>95</v>
+      <c r="A11" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="28"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>95</v>
+      <c r="A12" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>95</v>
+      <c r="A13" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>95</v>
+      <c r="A14" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>95</v>
+      <c r="A15" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E16" s="24" t="s">
+      <c r="A16" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E17" s="24" t="s">
+      <c r="A17" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" s="21" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2408,54 +2500,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" s="23" t="s">
+      <c r="C1" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="20" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="84" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>95</v>
+      <c r="A2" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>95</v>
+      <c r="A3" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>90</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>